<commit_message>
updated code for newer version of excelerize
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="JDE" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -131,6 +131,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -216,10 +217,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="F1:H31"/>
+  <dimension ref="C1:E31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -228,343 +229,343 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="1" t="n">
+      <c r="C2" s="1" t="n">
         <v>43466</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="1" t="n">
+      <c r="C3" s="1" t="n">
         <v>43467</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>-50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F4" s="1" t="n">
+      <c r="C4" s="1" t="n">
         <v>43468</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="1" t="n">
+      <c r="C5" s="1" t="n">
         <v>43469</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="E5" s="0" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="1" t="n">
+      <c r="C6" s="1" t="n">
         <v>43470</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="E6" s="0" t="n">
         <v>250</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="1" t="n">
+      <c r="C7" s="1" t="n">
         <v>43471</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="E7" s="0" t="n">
         <v>-250</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="1" t="n">
+      <c r="C8" s="1" t="n">
         <v>43472</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>350</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="1" t="n">
+      <c r="C9" s="1" t="n">
         <v>43473</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="E9" s="0" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="1" t="n">
+      <c r="C10" s="1" t="n">
         <v>43474</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="1" t="n">
+      <c r="C11" s="1" t="n">
         <v>43475</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="E11" s="0" t="n">
         <v>-450</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="1" t="n">
+      <c r="C12" s="1" t="n">
         <v>43476</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>550</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="1" t="n">
+      <c r="C13" s="1" t="n">
         <v>43477</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>-550</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="1" t="n">
+      <c r="C14" s="1" t="n">
         <v>43478</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="E14" s="0" t="n">
         <v>650</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="1" t="n">
+      <c r="C15" s="1" t="n">
         <v>43479</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="E15" s="0" t="n">
         <v>700</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="1" t="n">
+      <c r="C16" s="1" t="n">
         <v>43480</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="D16" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>750</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="1" t="n">
+      <c r="C17" s="1" t="n">
         <v>43481</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="E17" s="0" t="n">
         <v>800</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="1" t="n">
+      <c r="C18" s="1" t="n">
         <v>43482</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="E18" s="0" t="n">
         <v>850</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="1" t="n">
+      <c r="C19" s="1" t="n">
         <v>43483</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="D19" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="E19" s="0" t="n">
         <v>-850</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="1" t="n">
+      <c r="C20" s="1" t="n">
         <v>43484</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="E20" s="0" t="n">
         <v>950</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="1" t="n">
+      <c r="C21" s="1" t="n">
         <v>43485</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="E21" s="0" t="n">
         <v>1000</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="1" t="n">
+      <c r="C22" s="1" t="n">
         <v>43486</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="D22" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="E22" s="0" t="n">
         <v>1050</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="1" t="n">
+      <c r="C23" s="1" t="n">
         <v>43487</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="D23" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="E23" s="0" t="n">
         <v>1100</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="1" t="n">
+      <c r="C24" s="1" t="n">
         <v>43488</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="E24" s="0" t="n">
         <v>1150</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="1" t="n">
+      <c r="C25" s="1" t="n">
         <v>43489</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="D25" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="E25" s="0" t="n">
         <v>-1150</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="1" t="n">
+      <c r="C26" s="1" t="n">
         <v>43490</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="D26" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="E26" s="0" t="n">
         <v>1250</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="1" t="n">
+      <c r="C27" s="1" t="n">
         <v>43491</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="D27" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="E27" s="0" t="n">
         <v>1300</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="1" t="n">
+      <c r="C28" s="1" t="n">
         <v>43492</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="D28" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="E28" s="0" t="n">
         <v>1350</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="1" t="n">
+      <c r="C29" s="1" t="n">
         <v>43493</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="D29" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="E29" s="0" t="n">
         <v>-1350</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="1" t="n">
+      <c r="C30" s="1" t="n">
         <v>43494</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="D30" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="E30" s="0" t="n">
         <v>1450</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="1" t="n">
+      <c r="C31" s="1" t="n">
         <v>43495</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="E31" s="0" t="n">
         <v>1500</v>
       </c>
     </row>

</xml_diff>